<commit_message>
added bilinear interpolation. and also forward and backward 1d interpolations (trivial but sometimes useful for example in time series)
</commit_message>
<xml_diff>
--- a/ACQ.Excel/Demo.xlsx
+++ b/ACQ.Excel/Demo.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="5378"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="5378" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interpolation" sheetId="2" r:id="rId1"/>
-    <sheet name="Utils" sheetId="3" r:id="rId2"/>
+    <sheet name="Interpolaton2D" sheetId="4" r:id="rId2"/>
+    <sheet name="Utils" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>x</t>
   </si>
@@ -165,13 +166,29 @@
   <si>
     <t>dy2</t>
   </si>
+  <si>
+    <t>bilinear</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>2D interpolation using handle</t>
+  </si>
+  <si>
+    <t>2D interpolation in place</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -233,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,8 +272,20 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -375,6 +404,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -383,7 +591,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -401,9 +609,34 @@
     <xf numFmtId="14" fontId="7" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -435,6 +668,8 @@
         <stp>2e0596c6-8c62-47b9-b1cb-c5c4ba2e0617</stp>
         <tr r="P2" s="2"/>
       </tp>
+    </main>
+    <main first="rtdsrv.3324811a8f2a4b9eb5455293e7fec096">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
@@ -447,8 +682,6 @@
         <stp>63237a9d-3571-49a2-849e-3a24d01c6aaf</stp>
         <tr r="N2" s="2"/>
       </tp>
-    </main>
-    <main first="rtdsrv.3324811a8f2a4b9eb5455293e7fec096">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
@@ -461,6 +694,16 @@
         <stp>4e059e69-e1b4-4dea-bf1d-8ebc28e7a0d0</stp>
         <tr r="R2" s="2"/>
       </tp>
+    </main>
+    <main first="rtdsrv.63e2e7cd33ba4108924fb25473fe19ee">
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>564fcce3-2469-4c16-8bc9-f3726d31fdc7</stp>
+        <tr r="I4" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3324811a8f2a4b9eb5455293e7fec096">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
@@ -5852,6 +6095,2885 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="90"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9820190386649428E-2"/>
+          <c:y val="7.3369593310501233E-2"/>
+          <c:w val="0.87638114228891029"/>
+          <c:h val="0.80521581535951947"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:surfaceChart>
+        <c:wireframe val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$5:$V$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$6:$V$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84800000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59400000000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$7:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78799999999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.752</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$8:$V$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70400000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70800000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$9:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61599999999999988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63200000000000012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64799999999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68399999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68800000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69600000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$10:$V$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$11:$V$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.48800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57600000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.76400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$12:$V$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.79800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$13:$V$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27199999999999991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34400000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41599999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83200000000000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$14:$V$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35799999999999987</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.61399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$15:$V$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-7FB9-4FFA-84EC-D8CDFEEE96ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:bandFmts>
+          <c:bandFmt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="11"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="13"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="14"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+        </c:bandFmts>
+        <c:axId val="261643903"/>
+        <c:axId val="261634751"/>
+        <c:axId val="248543359"/>
+      </c:surfaceChart>
+      <c:catAx>
+        <c:axId val="261643903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="261634751"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="261634751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="261643903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="248543359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="261634751"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.5664260717410323E-2"/>
+          <c:y val="6.9444444444444448E-2"/>
+          <c:w val="0.88073862642169731"/>
+          <c:h val="0.73577136191309422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$5:$V$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3C80-49C7-A016-0FA5FECC4CC9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$6:$V$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84800000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59400000000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-10AC-4D3B-B303-9F8B93C070FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Interpolaton2D!$K$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$7:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78799999999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.752</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-10AC-4D3B-B303-9F8B93C070FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="94794271"/>
+        <c:axId val="94807583"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="94794271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94807583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="94807583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94794271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5975,6 +9097,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>54768</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635793</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6282,8 +9469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6325,10 +9512,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="19"/>
       <c r="M2" t="str">
         <f>_xll.acq_interpolator_create($B$4:$B$16,$C$4:$C$16,M$1,$F$4)</f>
         <v>#Interpolator:137</v>
@@ -13406,6 +16593,1184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:V28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.9296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="H4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f>_xll.acq_interpolator2d_create(D5:F5,C6:C7,D6:F7,I3)</f>
+        <v>#Interpolator2D:2</v>
+      </c>
+      <c r="L4" s="15">
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="N4" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="O4" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="P4" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="R4" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="S4" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="T4" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="U4" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="V4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="28">
+        <v>0</v>
+      </c>
+      <c r="E5" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="30">
+        <v>1</v>
+      </c>
+      <c r="K5" s="34">
+        <v>0</v>
+      </c>
+      <c r="L5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K5)</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K5)</f>
+        <v>0.96</v>
+      </c>
+      <c r="N5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K5)</f>
+        <v>0.92</v>
+      </c>
+      <c r="O5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K5)</f>
+        <v>0.88</v>
+      </c>
+      <c r="P5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K5)</f>
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="Q5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K5)</f>
+        <v>0.8</v>
+      </c>
+      <c r="R5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K5)</f>
+        <v>0.74</v>
+      </c>
+      <c r="S5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K5)</f>
+        <v>0.68</v>
+      </c>
+      <c r="T5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K5)</f>
+        <v>0.62</v>
+      </c>
+      <c r="U5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K5)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="V5" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K5)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="B6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="31">
+        <v>0</v>
+      </c>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="L6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K6)</f>
+        <v>0.9</v>
+      </c>
+      <c r="M6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K6)</f>
+        <v>0.874</v>
+      </c>
+      <c r="N6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K6)</f>
+        <v>0.84800000000000009</v>
+      </c>
+      <c r="O6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K6)</f>
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="P6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K6)</f>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="Q6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K6)</f>
+        <v>0.77</v>
+      </c>
+      <c r="R6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K6)</f>
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="S6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K6)</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="T6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K6)</f>
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="U6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K6)</f>
+        <v>0.59400000000000008</v>
+      </c>
+      <c r="V6" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K6)</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="20"/>
+      <c r="C7" s="32">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="K7" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K7)</f>
+        <v>0.8</v>
+      </c>
+      <c r="M7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K7)</f>
+        <v>0.78799999999999992</v>
+      </c>
+      <c r="N7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K7)</f>
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="O7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K7)</f>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="P7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K7)</f>
+        <v>0.752</v>
+      </c>
+      <c r="Q7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K7)</f>
+        <v>0.74</v>
+      </c>
+      <c r="R7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K7)</f>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="S7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K7)</f>
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="T7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K7)</f>
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="U7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K7)</f>
+        <v>0.628</v>
+      </c>
+      <c r="V7" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K7)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="B8" s="18"/>
+      <c r="K8" s="34">
+        <v>0.3</v>
+      </c>
+      <c r="L8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K8)</f>
+        <v>0.7</v>
+      </c>
+      <c r="M8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K8)</f>
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="N8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K8)</f>
+        <v>0.70400000000000007</v>
+      </c>
+      <c r="O8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K8)</f>
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="P8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K8)</f>
+        <v>0.70800000000000007</v>
+      </c>
+      <c r="Q8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K8)</f>
+        <v>0.71000000000000008</v>
+      </c>
+      <c r="R8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K8)</f>
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="S8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K8)</f>
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="T8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K8)</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="U8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K8)</f>
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="V8" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K8)</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="K9" s="34">
+        <v>0.4</v>
+      </c>
+      <c r="L9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K9)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K9)</f>
+        <v>0.61599999999999988</v>
+      </c>
+      <c r="N9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K9)</f>
+        <v>0.63200000000000012</v>
+      </c>
+      <c r="O9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K9)</f>
+        <v>0.64799999999999991</v>
+      </c>
+      <c r="P9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K9)</f>
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="Q9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K9)</f>
+        <v>0.68</v>
+      </c>
+      <c r="R9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K9)</f>
+        <v>0.68399999999999994</v>
+      </c>
+      <c r="S9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K9)</f>
+        <v>0.68800000000000006</v>
+      </c>
+      <c r="T9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K9)</f>
+        <v>0.69200000000000006</v>
+      </c>
+      <c r="U9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K9)</f>
+        <v>0.69600000000000006</v>
+      </c>
+      <c r="V9" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K9)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="K10" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K10)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K10)</f>
+        <v>0.53</v>
+      </c>
+      <c r="N10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K10)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K10)</f>
+        <v>0.59</v>
+      </c>
+      <c r="P10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K10)</f>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="Q10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K10)</f>
+        <v>0.65</v>
+      </c>
+      <c r="R10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K10)</f>
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="S10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K10)</f>
+        <v>0.69</v>
+      </c>
+      <c r="T10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K10)</f>
+        <v>0.71</v>
+      </c>
+      <c r="U10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K10)</f>
+        <v>0.73</v>
+      </c>
+      <c r="V10" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K10)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="K11" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="L11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K11)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K11)</f>
+        <v>0.44399999999999995</v>
+      </c>
+      <c r="N11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K11)</f>
+        <v>0.48800000000000004</v>
+      </c>
+      <c r="O11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K11)</f>
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="P11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K11)</f>
+        <v>0.57600000000000007</v>
+      </c>
+      <c r="Q11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K11)</f>
+        <v>0.62</v>
+      </c>
+      <c r="R11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K11)</f>
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="S11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K11)</f>
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="T11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K11)</f>
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="U11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K11)</f>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="V11" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K11)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="K12" s="34">
+        <v>0.7</v>
+      </c>
+      <c r="L12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K12)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="M12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K12)</f>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="N12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K12)</f>
+        <v>0.41600000000000004</v>
+      </c>
+      <c r="O12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K12)</f>
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="P12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K12)</f>
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="Q12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K12)</f>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="R12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K12)</f>
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="S12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K12)</f>
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="T12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K12)</f>
+        <v>0.746</v>
+      </c>
+      <c r="U12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K12)</f>
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="V12" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K12)</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="K13" s="34">
+        <v>0.8</v>
+      </c>
+      <c r="L13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K13)</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="M13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K13)</f>
+        <v>0.27199999999999991</v>
+      </c>
+      <c r="N13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K13)</f>
+        <v>0.34400000000000008</v>
+      </c>
+      <c r="O13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K13)</f>
+        <v>0.41599999999999993</v>
+      </c>
+      <c r="P13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K13)</f>
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="Q13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K13)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K13)</f>
+        <v>0.628</v>
+      </c>
+      <c r="S13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K13)</f>
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="T13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K13)</f>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="U13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K13)</f>
+        <v>0.83200000000000007</v>
+      </c>
+      <c r="V13" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K13)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="K14" s="34">
+        <v>0.9</v>
+      </c>
+      <c r="L14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K14)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="M14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K14)</f>
+        <v>0.18599999999999994</v>
+      </c>
+      <c r="N14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K14)</f>
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="O14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K14)</f>
+        <v>0.35799999999999987</v>
+      </c>
+      <c r="P14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K14)</f>
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="Q14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K14)</f>
+        <v>0.53</v>
+      </c>
+      <c r="R14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K14)</f>
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="S14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K14)</f>
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="T14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K14)</f>
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="U14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K14)</f>
+        <v>0.8660000000000001</v>
+      </c>
+      <c r="V14" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K14)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="K15" s="34">
+        <v>1</v>
+      </c>
+      <c r="L15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K15)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K15)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="N15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K15)</f>
+        <v>0.20000000000000007</v>
+      </c>
+      <c r="O15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K15)</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="P15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K15)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="R15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K15)</f>
+        <v>0.6</v>
+      </c>
+      <c r="S15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K15)</f>
+        <v>0.7</v>
+      </c>
+      <c r="T15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K15)</f>
+        <v>0.8</v>
+      </c>
+      <c r="U15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K15)</f>
+        <v>0.9</v>
+      </c>
+      <c r="V15" s="16">
+        <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="K17" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L18" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>1</v>
+      </c>
+      <c r="M18" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.96</v>
+      </c>
+      <c r="N18" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.92</v>
+      </c>
+      <c r="O18" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.88</v>
+      </c>
+      <c r="P18" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="Q18" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.8</v>
+      </c>
+      <c r="R18" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.74</v>
+      </c>
+      <c r="S18" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.68</v>
+      </c>
+      <c r="T18" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.62</v>
+      </c>
+      <c r="U18" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="V18" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L19" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.9</v>
+      </c>
+      <c r="M19" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.874</v>
+      </c>
+      <c r="N19" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.84800000000000009</v>
+      </c>
+      <c r="O19" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="P19" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="Q19" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.77</v>
+      </c>
+      <c r="R19" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="S19" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="T19" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="U19" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.59400000000000008</v>
+      </c>
+      <c r="V19" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L20" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.8</v>
+      </c>
+      <c r="M20" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.78799999999999992</v>
+      </c>
+      <c r="N20" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="O20" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="P20" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.752</v>
+      </c>
+      <c r="Q20" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.74</v>
+      </c>
+      <c r="R20" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="S20" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="T20" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="U20" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.628</v>
+      </c>
+      <c r="V20" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L21" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.7</v>
+      </c>
+      <c r="M21" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="N21" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.70400000000000007</v>
+      </c>
+      <c r="O21" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="P21" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.70800000000000007</v>
+      </c>
+      <c r="Q21" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.71000000000000008</v>
+      </c>
+      <c r="R21" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="S21" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="T21" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="U21" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="V21" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="22" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L22" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M22" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.61599999999999988</v>
+      </c>
+      <c r="N22" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.63200000000000012</v>
+      </c>
+      <c r="O22" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.64799999999999991</v>
+      </c>
+      <c r="P22" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="Q22" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.68</v>
+      </c>
+      <c r="R22" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.68399999999999994</v>
+      </c>
+      <c r="S22" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.68800000000000006</v>
+      </c>
+      <c r="T22" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69200000000000006</v>
+      </c>
+      <c r="U22" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69600000000000006</v>
+      </c>
+      <c r="V22" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L23" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M23" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.53</v>
+      </c>
+      <c r="N23" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O23" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.59</v>
+      </c>
+      <c r="P23" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="Q23" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.65</v>
+      </c>
+      <c r="R23" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="S23" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69</v>
+      </c>
+      <c r="T23" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.71</v>
+      </c>
+      <c r="U23" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.73</v>
+      </c>
+      <c r="V23" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L24" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M24" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.44399999999999995</v>
+      </c>
+      <c r="N24" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.48800000000000004</v>
+      </c>
+      <c r="O24" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="P24" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.57600000000000007</v>
+      </c>
+      <c r="Q24" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.62</v>
+      </c>
+      <c r="R24" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="S24" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="T24" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="U24" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="V24" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L25" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="M25" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="N25" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.41600000000000004</v>
+      </c>
+      <c r="O25" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="P25" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="Q25" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="R25" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="S25" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="T25" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.746</v>
+      </c>
+      <c r="U25" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="V25" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="26" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L26" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="M26" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.27199999999999991</v>
+      </c>
+      <c r="N26" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.34400000000000008</v>
+      </c>
+      <c r="O26" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.41599999999999993</v>
+      </c>
+      <c r="P26" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="Q26" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R26" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.628</v>
+      </c>
+      <c r="S26" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="T26" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="U26" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.83200000000000007</v>
+      </c>
+      <c r="V26" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L27" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="M27" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.18599999999999994</v>
+      </c>
+      <c r="N27" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="O27" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.35799999999999987</v>
+      </c>
+      <c r="P27" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="Q27" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.53</v>
+      </c>
+      <c r="R27" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="S27" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="T27" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="U27" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.8660000000000001</v>
+      </c>
+      <c r="V27" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="28" spans="11:22" x14ac:dyDescent="0.45">
+      <c r="L28" s="16">
+        <f>_xll.acq_interpolation2d(L$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="16">
+        <f>_xll.acq_interpolation2d(M$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="N28" s="16">
+        <f>_xll.acq_interpolation2d(N$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.20000000000000007</v>
+      </c>
+      <c r="O28" s="16">
+        <f>_xll.acq_interpolation2d(O$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="P28" s="16">
+        <f>_xll.acq_interpolation2d(P$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q28" s="16">
+        <f>_xll.acq_interpolation2d(Q$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.5</v>
+      </c>
+      <c r="R28" s="16">
+        <f>_xll.acq_interpolation2d(R$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="S28" s="16">
+        <f>_xll.acq_interpolation2d(S$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.7</v>
+      </c>
+      <c r="T28" s="16">
+        <f>_xll.acq_interpolation2d(T$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.8</v>
+      </c>
+      <c r="U28" s="16">
+        <f>_xll.acq_interpolation2d(U$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>0.9</v>
+      </c>
+      <c r="V28" s="16">
+        <f>_xll.acq_interpolation2d(V$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>